<commit_message>
Testing with updated masterdata file
</commit_message>
<xml_diff>
--- a/SS24 Pre Wood Wood import.xlsx
+++ b/SS24 Pre Wood Wood import.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://husethoyer.sharepoint.com/sites/MasterData/Delte dokumenter/General/WOOD WOOD/SS24 PRE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="194" documentId="8_{4A566DF7-3E5C-4B77-B2C0-2B924AABA208}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BB24F04A-3ADC-9847-90DF-5FD27DB6F52A}"/>
+  <xr:revisionPtr revIDLastSave="202" documentId="8_{4A566DF7-3E5C-4B77-B2C0-2B924AABA208}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{346F46B5-E684-8742-A36B-8DB5930665B9}"/>
   <bookViews>
-    <workbookView xWindow="9620" yWindow="500" windowWidth="40500" windowHeight="26340" xr2:uid="{6488FA1E-07FC-4508-9D43-18130FF5BB4D}"/>
+    <workbookView xWindow="3620" yWindow="8460" windowWidth="30240" windowHeight="16940" xr2:uid="{6488FA1E-07FC-4508-9D43-18130FF5BB4D}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">List1!$A$1:$AA$188</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +30,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1278,7 +1277,7 @@
   <dimension ref="A1:AA188"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1422,7 +1421,7 @@
         <v>270</v>
       </c>
       <c r="L2">
-        <v>517.69000000000005</v>
+        <v>528.25</v>
       </c>
       <c r="M2">
         <v>1399</v>
@@ -1489,7 +1488,7 @@
         <v>270</v>
       </c>
       <c r="L3">
-        <v>517.69000000000005</v>
+        <v>528.25</v>
       </c>
       <c r="M3">
         <v>1399</v>
@@ -1556,7 +1555,7 @@
         <v>270</v>
       </c>
       <c r="L4">
-        <v>517.69000000000005</v>
+        <v>528.25</v>
       </c>
       <c r="M4">
         <v>1399</v>
@@ -1623,7 +1622,7 @@
         <v>270</v>
       </c>
       <c r="L5">
-        <v>517.69000000000005</v>
+        <v>528.25</v>
       </c>
       <c r="M5">
         <v>1399</v>
@@ -1690,7 +1689,7 @@
         <v>270</v>
       </c>
       <c r="L6">
-        <v>517.69000000000005</v>
+        <v>528.25</v>
       </c>
       <c r="M6">
         <v>1399</v>
@@ -1757,7 +1756,7 @@
         <v>270</v>
       </c>
       <c r="L7">
-        <v>517.69000000000005</v>
+        <v>528.25</v>
       </c>
       <c r="M7">
         <v>1399</v>
@@ -1824,7 +1823,7 @@
         <v>270</v>
       </c>
       <c r="L8">
-        <v>517.69000000000005</v>
+        <v>528.25</v>
       </c>
       <c r="M8">
         <v>1399</v>
@@ -1891,7 +1890,7 @@
         <v>270</v>
       </c>
       <c r="L9">
-        <v>517.69000000000005</v>
+        <v>528.25</v>
       </c>
       <c r="M9">
         <v>1399</v>
@@ -1958,7 +1957,7 @@
         <v>270</v>
       </c>
       <c r="L10">
-        <v>517.69000000000005</v>
+        <v>528.25</v>
       </c>
       <c r="M10">
         <v>1399</v>
@@ -2025,7 +2024,7 @@
         <v>270</v>
       </c>
       <c r="L11">
-        <v>517.69000000000005</v>
+        <v>528.25</v>
       </c>
       <c r="M11">
         <v>1399</v>
@@ -2092,7 +2091,7 @@
         <v>270</v>
       </c>
       <c r="L12">
-        <v>517.69000000000005</v>
+        <v>528.25</v>
       </c>
       <c r="M12">
         <v>1399</v>
@@ -2159,7 +2158,7 @@
         <v>270</v>
       </c>
       <c r="L13">
-        <v>517.69000000000005</v>
+        <v>528.25</v>
       </c>
       <c r="M13">
         <v>1399</v>
@@ -2226,7 +2225,7 @@
         <v>270</v>
       </c>
       <c r="L14">
-        <v>517.69000000000005</v>
+        <v>528.25</v>
       </c>
       <c r="M14">
         <v>1399</v>
@@ -2293,7 +2292,7 @@
         <v>270</v>
       </c>
       <c r="L15">
-        <v>517.69000000000005</v>
+        <v>528.25</v>
       </c>
       <c r="M15">
         <v>1399</v>
@@ -2360,7 +2359,7 @@
         <v>270</v>
       </c>
       <c r="L16">
-        <v>517.69000000000005</v>
+        <v>528.25</v>
       </c>
       <c r="M16">
         <v>1399</v>
@@ -2427,7 +2426,7 @@
         <v>270</v>
       </c>
       <c r="L17">
-        <v>517.69000000000005</v>
+        <v>528.25</v>
       </c>
       <c r="M17">
         <v>1399</v>
@@ -2494,7 +2493,7 @@
         <v>270</v>
       </c>
       <c r="L18">
-        <v>517.69000000000005</v>
+        <v>528.25</v>
       </c>
       <c r="M18">
         <v>1399</v>
@@ -2561,7 +2560,7 @@
         <v>270</v>
       </c>
       <c r="L19">
-        <v>517.69000000000005</v>
+        <v>528.25</v>
       </c>
       <c r="M19">
         <v>1399</v>
@@ -2628,7 +2627,7 @@
         <v>270</v>
       </c>
       <c r="L20">
-        <v>443.7</v>
+        <v>452.75</v>
       </c>
       <c r="M20">
         <v>1199</v>
@@ -2695,7 +2694,7 @@
         <v>270</v>
       </c>
       <c r="L21">
-        <v>443.7</v>
+        <v>452.75</v>
       </c>
       <c r="M21">
         <v>1199</v>
@@ -2762,7 +2761,7 @@
         <v>270</v>
       </c>
       <c r="L22">
-        <v>443.7</v>
+        <v>452.75</v>
       </c>
       <c r="M22">
         <v>1199</v>
@@ -2829,7 +2828,7 @@
         <v>270</v>
       </c>
       <c r="L23">
-        <v>443.7</v>
+        <v>452.75</v>
       </c>
       <c r="M23">
         <v>1199</v>
@@ -2896,7 +2895,7 @@
         <v>270</v>
       </c>
       <c r="L24">
-        <v>443.7</v>
+        <v>452.75</v>
       </c>
       <c r="M24">
         <v>1199</v>
@@ -2963,7 +2962,7 @@
         <v>270</v>
       </c>
       <c r="L25">
-        <v>443.7</v>
+        <v>452.75</v>
       </c>
       <c r="M25">
         <v>1199</v>
@@ -3030,7 +3029,7 @@
         <v>270</v>
       </c>
       <c r="L26">
-        <v>443.7</v>
+        <v>452.75</v>
       </c>
       <c r="M26">
         <v>1199</v>
@@ -3097,7 +3096,7 @@
         <v>270</v>
       </c>
       <c r="L27">
-        <v>443.7</v>
+        <v>452.75</v>
       </c>
       <c r="M27">
         <v>1199</v>
@@ -3164,7 +3163,7 @@
         <v>270</v>
       </c>
       <c r="L28">
-        <v>443.7</v>
+        <v>452.75</v>
       </c>
       <c r="M28">
         <v>1199</v>
@@ -3231,7 +3230,7 @@
         <v>270</v>
       </c>
       <c r="L29">
-        <v>443.7</v>
+        <v>452.75</v>
       </c>
       <c r="M29">
         <v>1199</v>
@@ -3298,7 +3297,7 @@
         <v>270</v>
       </c>
       <c r="L30">
-        <v>517.69000000000005</v>
+        <v>528.25</v>
       </c>
       <c r="M30">
         <v>1399</v>
@@ -3365,7 +3364,7 @@
         <v>270</v>
       </c>
       <c r="L31">
-        <v>517.69000000000005</v>
+        <v>528.25</v>
       </c>
       <c r="M31">
         <v>1399</v>
@@ -3432,7 +3431,7 @@
         <v>270</v>
       </c>
       <c r="L32">
-        <v>517.69000000000005</v>
+        <v>528.25</v>
       </c>
       <c r="M32">
         <v>1399</v>
@@ -3499,7 +3498,7 @@
         <v>270</v>
       </c>
       <c r="L33">
-        <v>517.69000000000005</v>
+        <v>528.25</v>
       </c>
       <c r="M33">
         <v>1399</v>
@@ -3566,7 +3565,7 @@
         <v>270</v>
       </c>
       <c r="L34">
-        <v>517.69000000000005</v>
+        <v>528.25</v>
       </c>
       <c r="M34">
         <v>1399</v>
@@ -3968,7 +3967,7 @@
         <v>270</v>
       </c>
       <c r="L40">
-        <v>93.1</v>
+        <v>95</v>
       </c>
       <c r="M40">
         <v>299</v>
@@ -4035,7 +4034,7 @@
         <v>270</v>
       </c>
       <c r="L41">
-        <v>93.1</v>
+        <v>95</v>
       </c>
       <c r="M41">
         <v>299</v>
@@ -4102,7 +4101,7 @@
         <v>270</v>
       </c>
       <c r="L42">
-        <v>93.1</v>
+        <v>95</v>
       </c>
       <c r="M42">
         <v>299</v>
@@ -4169,7 +4168,7 @@
         <v>270</v>
       </c>
       <c r="L43">
-        <v>93.1</v>
+        <v>95</v>
       </c>
       <c r="M43">
         <v>299</v>
@@ -4504,7 +4503,7 @@
         <v>271</v>
       </c>
       <c r="L48">
-        <v>665.42</v>
+        <v>679</v>
       </c>
       <c r="M48">
         <v>1799</v>
@@ -4571,7 +4570,7 @@
         <v>271</v>
       </c>
       <c r="L49">
-        <v>665.42</v>
+        <v>679</v>
       </c>
       <c r="M49">
         <v>1799</v>
@@ -4638,7 +4637,7 @@
         <v>271</v>
       </c>
       <c r="L50">
-        <v>665.42</v>
+        <v>679</v>
       </c>
       <c r="M50">
         <v>1799</v>
@@ -5174,7 +5173,7 @@
         <v>271</v>
       </c>
       <c r="L58">
-        <v>554.67999999999995</v>
+        <v>566</v>
       </c>
       <c r="M58">
         <v>1499</v>
@@ -5241,7 +5240,7 @@
         <v>271</v>
       </c>
       <c r="L59">
-        <v>554.67999999999995</v>
+        <v>566</v>
       </c>
       <c r="M59">
         <v>1499</v>
@@ -5308,7 +5307,7 @@
         <v>271</v>
       </c>
       <c r="L60">
-        <v>554.67999999999995</v>
+        <v>566</v>
       </c>
       <c r="M60">
         <v>1499</v>
@@ -5844,7 +5843,7 @@
         <v>271</v>
       </c>
       <c r="L68">
-        <v>610.04999999999995</v>
+        <v>622.5</v>
       </c>
       <c r="M68">
         <v>1699</v>
@@ -5911,7 +5910,7 @@
         <v>271</v>
       </c>
       <c r="L69">
-        <v>610.04999999999995</v>
+        <v>622.5</v>
       </c>
       <c r="M69">
         <v>1699</v>
@@ -5978,7 +5977,7 @@
         <v>271</v>
       </c>
       <c r="L70">
-        <v>610.04999999999995</v>
+        <v>622.5</v>
       </c>
       <c r="M70">
         <v>1699</v>
@@ -6045,7 +6044,7 @@
         <v>271</v>
       </c>
       <c r="L71">
-        <v>610.04999999999995</v>
+        <v>622.5</v>
       </c>
       <c r="M71">
         <v>1699</v>
@@ -6715,7 +6714,7 @@
         <v>271</v>
       </c>
       <c r="L81">
-        <v>554.67999999999995</v>
+        <v>566</v>
       </c>
       <c r="M81">
         <v>1499</v>
@@ -6782,7 +6781,7 @@
         <v>271</v>
       </c>
       <c r="L82">
-        <v>554.67999999999995</v>
+        <v>566</v>
       </c>
       <c r="M82">
         <v>1499</v>
@@ -6849,7 +6848,7 @@
         <v>271</v>
       </c>
       <c r="L83">
-        <v>554.67999999999995</v>
+        <v>566</v>
       </c>
       <c r="M83">
         <v>1499</v>
@@ -6916,7 +6915,7 @@
         <v>271</v>
       </c>
       <c r="L84">
-        <v>554.67999999999995</v>
+        <v>566</v>
       </c>
       <c r="M84">
         <v>1499</v>
@@ -7251,7 +7250,7 @@
         <v>271</v>
       </c>
       <c r="L89">
-        <v>277.33999999999997</v>
+        <v>283</v>
       </c>
       <c r="M89">
         <v>749</v>
@@ -7318,7 +7317,7 @@
         <v>271</v>
       </c>
       <c r="L90">
-        <v>277.33999999999997</v>
+        <v>283</v>
       </c>
       <c r="M90">
         <v>749</v>
@@ -7385,7 +7384,7 @@
         <v>271</v>
       </c>
       <c r="L91">
-        <v>277.33999999999997</v>
+        <v>283</v>
       </c>
       <c r="M91">
         <v>749</v>
@@ -7452,7 +7451,7 @@
         <v>271</v>
       </c>
       <c r="L92">
-        <v>277.33999999999997</v>
+        <v>283</v>
       </c>
       <c r="M92">
         <v>749</v>
@@ -7519,7 +7518,7 @@
         <v>271</v>
       </c>
       <c r="L93">
-        <v>277.33999999999997</v>
+        <v>283</v>
       </c>
       <c r="M93">
         <v>749</v>
@@ -7586,7 +7585,7 @@
         <v>271</v>
       </c>
       <c r="L94">
-        <v>277.33999999999997</v>
+        <v>283</v>
       </c>
       <c r="M94">
         <v>749</v>
@@ -7653,7 +7652,7 @@
         <v>271</v>
       </c>
       <c r="L95">
-        <v>277.33999999999997</v>
+        <v>283</v>
       </c>
       <c r="M95">
         <v>749</v>
@@ -7720,7 +7719,7 @@
         <v>271</v>
       </c>
       <c r="L96">
-        <v>277.33999999999997</v>
+        <v>283</v>
       </c>
       <c r="M96">
         <v>749</v>
@@ -8993,10 +8992,10 @@
         <v>271</v>
       </c>
       <c r="L115">
-        <v>339.5</v>
+        <v>226.25</v>
       </c>
       <c r="M115">
-        <v>899</v>
+        <v>599</v>
       </c>
       <c r="O115" t="s">
         <v>52</v>
@@ -9060,10 +9059,10 @@
         <v>271</v>
       </c>
       <c r="L116">
-        <v>339.5</v>
+        <v>226.25</v>
       </c>
       <c r="M116">
-        <v>899</v>
+        <v>599</v>
       </c>
       <c r="O116" t="s">
         <v>52</v>
@@ -9127,10 +9126,10 @@
         <v>271</v>
       </c>
       <c r="L117">
-        <v>339.5</v>
+        <v>226.25</v>
       </c>
       <c r="M117">
-        <v>899</v>
+        <v>599</v>
       </c>
       <c r="O117" t="s">
         <v>52</v>
@@ -9194,10 +9193,10 @@
         <v>271</v>
       </c>
       <c r="L118">
-        <v>339.5</v>
+        <v>226.25</v>
       </c>
       <c r="M118">
-        <v>899</v>
+        <v>599</v>
       </c>
       <c r="O118" t="s">
         <v>52</v>
@@ -9395,7 +9394,7 @@
         <v>271</v>
       </c>
       <c r="L121">
-        <v>776.41</v>
+        <v>792.25</v>
       </c>
       <c r="M121">
         <v>2099</v>
@@ -9462,7 +9461,7 @@
         <v>271</v>
       </c>
       <c r="L122">
-        <v>776.41</v>
+        <v>792.25</v>
       </c>
       <c r="M122">
         <v>2099</v>
@@ -9529,7 +9528,7 @@
         <v>271</v>
       </c>
       <c r="L123">
-        <v>776.41</v>
+        <v>792.25</v>
       </c>
       <c r="M123">
         <v>2099</v>
@@ -9596,7 +9595,7 @@
         <v>271</v>
       </c>
       <c r="L124">
-        <v>776.41</v>
+        <v>792.25</v>
       </c>
       <c r="M124">
         <v>2099</v>
@@ -9663,7 +9662,7 @@
         <v>271</v>
       </c>
       <c r="L125">
-        <v>776.41</v>
+        <v>792.25</v>
       </c>
       <c r="M125">
         <v>2099</v>
@@ -9730,7 +9729,7 @@
         <v>271</v>
       </c>
       <c r="L126">
-        <v>776.41</v>
+        <v>792.25</v>
       </c>
       <c r="M126">
         <v>2099</v>
@@ -10199,7 +10198,7 @@
         <v>271</v>
       </c>
       <c r="L133">
-        <v>1109.3599999999999</v>
+        <v>1132</v>
       </c>
       <c r="M133">
         <v>2999</v>
@@ -10266,7 +10265,7 @@
         <v>271</v>
       </c>
       <c r="L134">
-        <v>1109.3599999999999</v>
+        <v>1132</v>
       </c>
       <c r="M134">
         <v>2999</v>
@@ -10333,7 +10332,7 @@
         <v>271</v>
       </c>
       <c r="L135">
-        <v>1109.3599999999999</v>
+        <v>1132</v>
       </c>
       <c r="M135">
         <v>2999</v>
@@ -10668,7 +10667,7 @@
         <v>271</v>
       </c>
       <c r="L140">
-        <v>554.67999999999995</v>
+        <v>566</v>
       </c>
       <c r="M140">
         <v>1499</v>
@@ -10735,7 +10734,7 @@
         <v>271</v>
       </c>
       <c r="L141">
-        <v>554.67999999999995</v>
+        <v>566</v>
       </c>
       <c r="M141">
         <v>1499</v>
@@ -10802,7 +10801,7 @@
         <v>271</v>
       </c>
       <c r="L142">
-        <v>554.67999999999995</v>
+        <v>566</v>
       </c>
       <c r="M142">
         <v>1499</v>
@@ -11070,7 +11069,7 @@
         <v>271</v>
       </c>
       <c r="L146">
-        <v>1053.75</v>
+        <v>1075.25</v>
       </c>
       <c r="M146">
         <v>2899</v>
@@ -11137,7 +11136,7 @@
         <v>271</v>
       </c>
       <c r="L147">
-        <v>1053.75</v>
+        <v>1075.25</v>
       </c>
       <c r="M147">
         <v>2899</v>
@@ -11204,7 +11203,7 @@
         <v>271</v>
       </c>
       <c r="L148">
-        <v>1053.75</v>
+        <v>1075.25</v>
       </c>
       <c r="M148">
         <v>2899</v>
@@ -11673,7 +11672,7 @@
         <v>271</v>
       </c>
       <c r="L155">
-        <v>332.71</v>
+        <v>339.5</v>
       </c>
       <c r="M155">
         <v>899</v>
@@ -11740,7 +11739,7 @@
         <v>271</v>
       </c>
       <c r="L156">
-        <v>332.71</v>
+        <v>339.5</v>
       </c>
       <c r="M156">
         <v>899</v>
@@ -11807,7 +11806,7 @@
         <v>271</v>
       </c>
       <c r="L157">
-        <v>332.71</v>
+        <v>339.5</v>
       </c>
       <c r="M157">
         <v>899</v>
@@ -11874,7 +11873,7 @@
         <v>271</v>
       </c>
       <c r="L158">
-        <v>332.71</v>
+        <v>339.5</v>
       </c>
       <c r="M158">
         <v>899</v>
@@ -12117,7 +12116,7 @@
         <v>90</v>
       </c>
       <c r="C162" t="str">
-        <f t="shared" ref="C162:C193" si="10">D162&amp;"-"&amp;H162</f>
+        <f t="shared" ref="C162:C188" si="10">D162&amp;"-"&amp;H162</f>
         <v xml:space="preserve">0001-White  </v>
       </c>
       <c r="D162" t="s">
@@ -12163,7 +12162,7 @@
         <v>287</v>
       </c>
       <c r="U162" t="str">
-        <f t="shared" ref="U162:U193" si="11">"Country of origin: "&amp;V162&amp;" / Composition: "&amp;W162</f>
+        <f t="shared" ref="U162:U188" si="11">"Country of origin: "&amp;V162&amp;" / Composition: "&amp;W162</f>
         <v>Country of origin: Portugal / Composition: 100% cotton (Organic)</v>
       </c>
       <c r="V162" t="s">
@@ -12477,7 +12476,7 @@
         <v>271</v>
       </c>
       <c r="L167">
-        <v>443.7</v>
+        <v>452.75</v>
       </c>
       <c r="M167">
         <v>1199</v>
@@ -12544,7 +12543,7 @@
         <v>271</v>
       </c>
       <c r="L168">
-        <v>443.7</v>
+        <v>452.75</v>
       </c>
       <c r="M168">
         <v>1199</v>
@@ -12611,7 +12610,7 @@
         <v>271</v>
       </c>
       <c r="L169">
-        <v>443.7</v>
+        <v>452.75</v>
       </c>
       <c r="M169">
         <v>1199</v>
@@ -12946,7 +12945,7 @@
         <v>271</v>
       </c>
       <c r="L174">
-        <v>776.41</v>
+        <v>792.25</v>
       </c>
       <c r="M174">
         <v>2099</v>
@@ -13013,7 +13012,7 @@
         <v>271</v>
       </c>
       <c r="L175">
-        <v>776.41</v>
+        <v>792.25</v>
       </c>
       <c r="M175">
         <v>2099</v>
@@ -13080,7 +13079,7 @@
         <v>271</v>
       </c>
       <c r="L176">
-        <v>776.41</v>
+        <v>792.25</v>
       </c>
       <c r="M176">
         <v>2099</v>
@@ -13147,7 +13146,7 @@
         <v>271</v>
       </c>
       <c r="L177">
-        <v>776.41</v>
+        <v>792.25</v>
       </c>
       <c r="M177">
         <v>2099</v>
@@ -13214,7 +13213,7 @@
         <v>271</v>
       </c>
       <c r="L178">
-        <v>776.41</v>
+        <v>792.25</v>
       </c>
       <c r="M178">
         <v>2099</v>
@@ -13281,7 +13280,7 @@
         <v>271</v>
       </c>
       <c r="L179">
-        <v>776.41</v>
+        <v>792.25</v>
       </c>
       <c r="M179">
         <v>2099</v>
@@ -13348,7 +13347,7 @@
         <v>271</v>
       </c>
       <c r="L180">
-        <v>776.41</v>
+        <v>792.25</v>
       </c>
       <c r="M180">
         <v>2099</v>
@@ -14171,22 +14170,22 @@
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{669DCF39-F382-45B5-842F-A4F67AE395DB}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="0ef2e197-08a6-455d-9799-208287a7b48d"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="c99395ac-0055-47c5-89f6-537638cb2d4f"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="c99395ac-0055-47c5-89f6-537638cb2d4f"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{34EE1B64-0EBD-481E-9715-9706CFA2BA21}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B48C04C5-73C6-4578-8A37-ECE481E9BE9E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>

</xml_diff>